<commit_message>
clean folder and add test file
</commit_message>
<xml_diff>
--- a/[test]PayRecon - MY - ScanBulk Upload.xlsx
+++ b/[test]PayRecon - MY - ScanBulk Upload.xlsx
@@ -5,12 +5,12 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lwsee\Downloads\Chrome\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lwsee\Documents\Python\230917_Payrecon_Concat_Sort_Clean\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6F03F36-0D4B-4497-B433-C72CF7D6888B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD1902EB-08EF-4E03-9720-B7E70305636D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1884" yWindow="1884" windowWidth="23040" windowHeight="12204" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="58575" yWindow="1920" windowWidth="21825" windowHeight="15600" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -233,7 +233,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -589,10 +589,10 @@
   <dimension ref="A1:R10"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="19.44140625" customWidth="1"/>
     <col min="3" max="5" width="24.6640625" customWidth="1"/>
@@ -610,7 +610,7 @@
     <col min="18" max="18" width="52" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -632,7 +632,7 @@
       <c r="Q1" s="4"/>
       <c r="R1" s="4"/>
     </row>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -685,7 +685,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>407247400621848</v>
       </c>
@@ -726,7 +726,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:18">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>407194282151122</v>
       </c>
@@ -767,7 +767,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:18">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>407193440244068</v>
       </c>
@@ -808,7 +808,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:18">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>407171836132070</v>
       </c>
@@ -849,7 +849,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:18">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>409609924514235</v>
       </c>
@@ -890,7 +890,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:18">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>409605526355498</v>
       </c>
@@ -931,7 +931,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="9" spans="1:18">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>409573378836252</v>
       </c>
@@ -963,7 +963,7 @@
         <v>25</v>
       </c>
       <c r="M9" s="2">
-        <v>600177235028</v>
+        <v>60177235028</v>
       </c>
       <c r="Q9" t="s">
         <v>62</v>
@@ -972,7 +972,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="10" spans="1:18">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>409588712996067</v>
       </c>

</xml_diff>